<commit_message>
removed from FNDIV_final_project folder
</commit_message>
<xml_diff>
--- a/data_spreadsheet.xlsx
+++ b/data_spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/School/PhD/Courses/Spring2025_Foundations_4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/School/Documents/GitHub/FNDIV_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2618BFD4-9C8B-7044-B92B-732F1DFF1EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC35B21-943A-FF46-BC50-7A8F5CD2F4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{F7D63427-C7E1-4A49-A339-88C46ECA8192}"/>
   </bookViews>
@@ -2987,7 +2987,7 @@
   <dimension ref="A1:AV85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A1:AV85"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15623,6 +15623,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2d59f02d-5893-4320-bddc-4676827c17eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF89177CE8279B47A0F1724028094282" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2132eff01d5c50140375705bf09781b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2d59f02d-5893-4320-bddc-4676827c17eb" xmlns:ns4="5d0410f2-bef2-4ee6-8a3e-fae655e7a71c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ee9642b5b29b0a5c2ccd16a37de68e8" ns3:_="" ns4:_="">
     <xsd:import namespace="2d59f02d-5893-4320-bddc-4676827c17eb"/>
@@ -15863,24 +15880,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47D54D3A-2CE3-4066-AFBD-F94FF380D0A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2d59f02d-5893-4320-bddc-4676827c17eb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2d59f02d-5893-4320-bddc-4676827c17eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE8C058C-769E-4637-B019-DFADD9E10F8E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA1BD459-36DF-4548-AC40-21C2801ACD85}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15897,22 +15915,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE8C058C-769E-4637-B019-DFADD9E10F8E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47D54D3A-2CE3-4066-AFBD-F94FF380D0A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2d59f02d-5893-4320-bddc-4676827c17eb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>